<commit_message>
add the cliff tile and the resources #21
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Tile.xlsx
+++ b/ConfigData/Xlsx/Tile.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Tile" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>water</t>
   </si>
@@ -138,13 +143,69 @@
   </si>
   <si>
     <t>Color</t>
+  </si>
+  <si>
+    <t>9|DefaultTile</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CanMove</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否可以移动</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>图标</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brown</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>悬崖</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fall</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,7 +816,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -763,28 +824,31 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -799,30 +863,44 @@
     <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E12" totalsRowShown="0">
-  <autoFilter ref="A1:E12"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:G13" totalsRowShown="0">
+  <autoFilter ref="A1:G13"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Cname"/>
     <tableColumn id="4" name="Type"/>
+    <tableColumn id="6" name="CanMove"/>
+    <tableColumn id="7" name="Icon" dataDxfId="0"/>
     <tableColumn id="5" name="Color"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -872,7 +950,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -904,9 +982,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -938,6 +1017,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1113,16 +1193,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1136,10 +1216,16 @@
         <v>37</v>
       </c>
       <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1153,10 +1239,16 @@
         <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -1170,10 +1262,16 @@
         <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1186,11 +1284,17 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1203,11 +1307,17 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1220,11 +1330,17 @@
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1237,11 +1353,17 @@
       <c r="D7">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1254,11 +1376,17 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1271,11 +1399,17 @@
       <c r="D9">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="3">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1288,11 +1422,17 @@
       <c r="D10">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="3">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1305,13 +1445,19 @@
       <c r="D11">
         <v>8</v>
       </c>
-      <c r="E11" t="s">
-        <v>23</v>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="3">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>9</v>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -1322,15 +1468,45 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>